<commit_message>
create many windows as add project and update project and link project with a datbase called product_DB
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -4,18 +4,93 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t>ID_cat</t>
+  </si>
+  <si>
+    <t>Describtion_Cat</t>
+  </si>
+  <si>
+    <t>Caregories</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>ID_Product</t>
+  </si>
+  <si>
+    <t>Label_Product</t>
+  </si>
+  <si>
+    <t>QTE_in_Stock</t>
+  </si>
+  <si>
+    <t>price )varchar)</t>
+  </si>
+  <si>
+    <t>image_Product image</t>
+  </si>
+  <si>
+    <t>ID_Cat</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>ID_Customer</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Tel (Ncahr(15)</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>image_Customer nvarchar(max)</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>ID_Order</t>
+  </si>
+  <si>
+    <t>Date_Order DateTime</t>
+  </si>
+  <si>
+    <t>Customer_ID</t>
+  </si>
+  <si>
+    <t>QTE</t>
+  </si>
+  <si>
+    <t>Orders_Details</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +406,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>